<commit_message>
Tambah 1 column data test modul 12
</commit_message>
<xml_diff>
--- a/Data Test Modul 12.xlsx
+++ b/Data Test Modul 12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MICHAEL\git\TEProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\git\ProjectTE-11-123\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE397646-EC52-40A3-B429-BF4ECE4D6A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B82C39C-7D49-4045-8009-30F14C0A14D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{25A1A1CD-DC07-4A8D-9351-81C7AACB944A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{25A1A1CD-DC07-4A8D-9351-81C7AACB944A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Nama Depan</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>hai</t>
+  </si>
+  <si>
+    <t>Nama Belakang</t>
+  </si>
+  <si>
+    <t>Hula</t>
+  </si>
+  <si>
+    <t>HUla</t>
   </si>
 </sst>
 </file>
@@ -399,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147F941C-CC38-453D-95B7-1C82BE184D5A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,30 +420,39 @@
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>